<commit_message>
Perbaikan bugs dpia controller
</commit_message>
<xml_diff>
--- a/PrivafoWeb/wwwroot/shared/UserFiles/Folders/sasa.xlsx
+++ b/PrivafoWeb/wwwroot/shared/UserFiles/Folders/sasa.xlsx
@@ -48,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
+    <xf numFmtId="1" fontId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,10 +170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="100" topLeftCell="A1" workbookViewId="0" showGridLines="true" showRowColHeaders="true">
-      <selection activeCell="D2" sqref="D2:D2"/>
+      <selection activeCell="F2" sqref="F2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="false" defaultColWidth="9.28125" defaultRowHeight="15"/>
@@ -181,6 +182,9 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1" t="n">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.6999999999999998" right="0.6999999999999998" top="0.75"/>

</xml_diff>